<commit_message>
Combining bubble charts into one
</commit_message>
<xml_diff>
--- a/word counts.xlsx
+++ b/word counts.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gurka\Desktop\deep-fiction\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{94ABFD3E-EC26-493B-A265-FDA7CB5FAA05}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6AB716A4-A147-4F1C-99A5-985E2A8B51AA}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="12480" yWindow="2316" windowWidth="8880" windowHeight="8964" activeTab="1" xr2:uid="{528B8027-8BB7-4F62-AC04-B1EA881BB4A8}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{528B8027-8BB7-4F62-AC04-B1EA881BB4A8}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="231" uniqueCount="131">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="225" uniqueCount="111">
   <si>
     <t>five letters</t>
   </si>
@@ -365,66 +365,6 @@
   </si>
   <si>
     <t>carefully</t>
-  </si>
-  <si>
-    <t xml:space="preserve">      ['Robert', ' Jordan'],</t>
-  </si>
-  <si>
-    <t xml:space="preserve">      ['Steven', ' Erikson'],</t>
-  </si>
-  <si>
-    <t xml:space="preserve">      ['George', ' R. R. Martin'],</t>
-  </si>
-  <si>
-    <t xml:space="preserve">      ['Brandon', 'Sanderson'],</t>
-  </si>
-  <si>
-    <t xml:space="preserve">      ['Stephen', 'King'],</t>
-  </si>
-  <si>
-    <t xml:space="preserve">      ['J. K.', 'Rowling'],</t>
-  </si>
-  <si>
-    <t xml:space="preserve">      ['Tad', 'Williams'],</t>
-  </si>
-  <si>
-    <t xml:space="preserve">      ['Stephen', 'R. Lawhead'],</t>
-  </si>
-  <si>
-    <t xml:space="preserve">      ['Patrick', 'Rothfuss'],</t>
-  </si>
-  <si>
-    <t xml:space="preserve">      ['J. R. R.', 'Tolkien'],</t>
-  </si>
-  <si>
-    <t xml:space="preserve">      ['Christopher', 'Paolini'],</t>
-  </si>
-  <si>
-    <t xml:space="preserve">      ['Joe', 'Abercrombie'],</t>
-  </si>
-  <si>
-    <t xml:space="preserve">      ['David', 'Eddings'],</t>
-  </si>
-  <si>
-    <t xml:space="preserve">      ['Scott', 'Bakker'],</t>
-  </si>
-  <si>
-    <t xml:space="preserve">      ['Gene', 'Wolfe'],</t>
-  </si>
-  <si>
-    <t xml:space="preserve">      ['Guy', 'Gavriel Kay'],</t>
-  </si>
-  <si>
-    <t xml:space="preserve">      ['Garth', 'Nix'],</t>
-  </si>
-  <si>
-    <t xml:space="preserve">      ['C. S.', 'Lewis'],</t>
-  </si>
-  <si>
-    <t xml:space="preserve">      ['Ursula', 'K Le Guin'],</t>
-  </si>
-  <si>
-    <t xml:space="preserve">      ['Fred', 'Saberhagen']</t>
   </si>
 </sst>
 </file>
@@ -445,7 +385,7 @@
       <name val="Arial Unicode MS"/>
     </font>
   </fonts>
-  <fills count="13">
+  <fills count="14">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -518,6 +458,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -531,7 +477,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -571,6 +517,11 @@
     <xf numFmtId="1" fontId="0" fillId="12" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="1" fontId="0" fillId="13" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -888,7 +839,7 @@
   <dimension ref="A1:Z56"/>
   <sheetViews>
     <sheetView topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="O1" sqref="O1:P11"/>
+      <selection activeCell="I1" sqref="I1:J11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -1120,7 +1071,7 @@
         <v>8</v>
       </c>
       <c r="L4">
-        <f t="shared" ref="L3:L11" si="2">(J4/MIN(J4:J13))*15</f>
+        <f t="shared" ref="L4:L11" si="2">(J4/MIN(J4:J13))*15</f>
         <v>30.625760761314595</v>
       </c>
       <c r="M4" s="1" t="s">
@@ -2363,16 +2314,17 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{69EC9610-E97A-4183-B2FB-9D4DB3A1EDAA}">
-  <dimension ref="A1:E60"/>
+  <dimension ref="A1:E68"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A33" workbookViewId="0">
-      <selection activeCell="A41" sqref="A41:A60"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E24" sqref="E24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="24.44140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.33203125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="7.44140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
@@ -2579,193 +2531,200 @@
         <v>35.526227782250572</v>
       </c>
     </row>
+    <row r="12" spans="1:5">
+      <c r="A12" s="19"/>
+      <c r="B12" s="20"/>
+      <c r="C12" s="20"/>
+      <c r="D12" s="21"/>
+      <c r="E12" s="20"/>
+    </row>
     <row r="13" spans="1:5">
-      <c r="A13" s="17" t="s">
-        <v>14</v>
-      </c>
-      <c r="B13" s="17" t="s">
+      <c r="A13" s="13" t="s">
+        <v>13</v>
+      </c>
+      <c r="B13" s="13" t="s">
         <v>11</v>
       </c>
-      <c r="C13" s="17" t="s">
+      <c r="C13" s="13" t="s">
         <v>62</v>
       </c>
-      <c r="D13" s="17" t="s">
+      <c r="D13" s="13" t="s">
         <v>60</v>
       </c>
-      <c r="E13" s="17"/>
+      <c r="E13" s="13"/>
     </row>
     <row r="14" spans="1:5">
       <c r="A14" s="14" t="s">
-        <v>41</v>
+        <v>31</v>
       </c>
       <c r="B14" s="15">
-        <v>8886</v>
+        <v>27717</v>
       </c>
       <c r="C14" s="15">
         <v>3</v>
       </c>
-      <c r="D14" s="15"/>
+      <c r="D14" s="16"/>
       <c r="E14" s="15">
-        <f>(B14/(MIN(B14:B23)))*20</f>
-        <v>37.708465945257799</v>
+        <f>(B14/(MIN(B14:B23)))*18</f>
+        <v>55.207037733761204</v>
       </c>
     </row>
     <row r="15" spans="1:5">
       <c r="A15" s="14" t="s">
-        <v>48</v>
+        <v>32</v>
       </c>
       <c r="B15" s="15">
-        <v>6520</v>
+        <v>25427</v>
       </c>
       <c r="C15" s="15">
         <f>(C14+3)</f>
         <v>6</v>
       </c>
-      <c r="D15" s="15"/>
+      <c r="D15" s="16"/>
       <c r="E15" s="15">
-        <f>(B15/(MIN(B14:B23)))*20</f>
-        <v>27.668151920220666</v>
+        <f>(B15/(MIN(B14:B23)))*18</f>
+        <v>50.645789531924315</v>
       </c>
     </row>
     <row r="16" spans="1:5">
       <c r="A16" s="14" t="s">
-        <v>42</v>
+        <v>33</v>
       </c>
       <c r="B16" s="15">
-        <v>5821</v>
+        <v>18451</v>
       </c>
       <c r="C16" s="15">
-        <f t="shared" ref="C16:C23" si="1">(C15+3)</f>
+        <f>(C15+3)</f>
         <v>9</v>
       </c>
-      <c r="D16" s="15"/>
+      <c r="D16" s="16"/>
       <c r="E16" s="15">
-        <f>(B16/(MIN(B14:B23)))*20</f>
-        <v>24.701888393804371</v>
+        <f>(B16/(MIN(B14:B23)))*18</f>
+        <v>36.750912913577515</v>
       </c>
     </row>
     <row r="17" spans="1:5">
       <c r="A17" s="14" t="s">
-        <v>43</v>
+        <v>34</v>
       </c>
       <c r="B17" s="15">
-        <v>5694</v>
+        <v>14941</v>
       </c>
       <c r="C17" s="15">
-        <f t="shared" si="1"/>
+        <f>(C16+3)</f>
         <v>12</v>
       </c>
-      <c r="D17" s="15"/>
+      <c r="D17" s="16"/>
       <c r="E17" s="15">
-        <f>(B17/(MIN(B14:B23)))*20</f>
-        <v>24.162953532781664</v>
+        <f>(B17/(MIN(B14:B23)))*18</f>
+        <v>29.759654752683414</v>
       </c>
     </row>
     <row r="18" spans="1:5">
       <c r="A18" s="14" t="s">
-        <v>44</v>
+        <v>35</v>
       </c>
       <c r="B18" s="15">
-        <v>5456</v>
+        <v>14934</v>
       </c>
       <c r="C18" s="15">
-        <f t="shared" si="1"/>
+        <f>(C17+3)</f>
         <v>15</v>
       </c>
-      <c r="D18" s="15"/>
+      <c r="D18" s="16"/>
       <c r="E18" s="15">
-        <f>(B18/(MIN(B14:B23)))*20</f>
-        <v>23.152981116061959</v>
+        <f>(B18/(MIN(B14:B23)))*18</f>
+        <v>29.745712072590461</v>
       </c>
     </row>
     <row r="19" spans="1:5">
       <c r="A19" s="14" t="s">
-        <v>45</v>
+        <v>36</v>
       </c>
       <c r="B19" s="15">
-        <v>5290</v>
+        <v>14600</v>
       </c>
       <c r="C19" s="15">
-        <f t="shared" si="1"/>
+        <f>(C18+3)</f>
         <v>18</v>
       </c>
-      <c r="D19" s="15"/>
+      <c r="D19" s="16"/>
       <c r="E19" s="15">
-        <f>(B19/(MIN(B14:B23)))*20</f>
-        <v>22.448546573307873</v>
+        <f>(B19/(MIN(B14:B23)))*18</f>
+        <v>29.080447051012502</v>
       </c>
     </row>
     <row r="20" spans="1:5">
       <c r="A20" s="14" t="s">
-        <v>46</v>
+        <v>37</v>
       </c>
       <c r="B20" s="15">
-        <v>5110</v>
+        <v>10743</v>
       </c>
       <c r="C20" s="15">
-        <f t="shared" si="1"/>
+        <f>(C19+3)</f>
         <v>21</v>
       </c>
-      <c r="D20" s="15"/>
+      <c r="D20" s="16"/>
       <c r="E20" s="15">
-        <f>(B20/(MIN(B14:B23)))*20</f>
-        <v>21.684701888393803</v>
+        <f>(B20/(MIN(B14:B23)))*18</f>
+        <v>21.398030319796391</v>
       </c>
     </row>
     <row r="21" spans="1:5">
       <c r="A21" s="14" t="s">
-        <v>47</v>
+        <v>38</v>
       </c>
       <c r="B21" s="15">
-        <v>4822</v>
+        <v>10628</v>
       </c>
       <c r="C21" s="15">
-        <f t="shared" si="1"/>
+        <f>(C20+3)</f>
         <v>24</v>
       </c>
-      <c r="D21" s="15"/>
+      <c r="D21" s="16"/>
       <c r="E21" s="15">
-        <f>(B21/(MIN(B14:B23)))*20</f>
-        <v>20.462550392531295</v>
+        <f>(B21/(MIN(B14:B23)))*18</f>
+        <v>21.168972003983626</v>
       </c>
     </row>
     <row r="22" spans="1:5">
       <c r="A22" s="14" t="s">
-        <v>49</v>
+        <v>39</v>
       </c>
       <c r="B22" s="15">
-        <v>4753</v>
+        <v>10478</v>
       </c>
       <c r="C22" s="15">
-        <f t="shared" si="1"/>
+        <f>(C21+3)</f>
         <v>27</v>
       </c>
-      <c r="D22" s="15"/>
+      <c r="D22" s="16"/>
       <c r="E22" s="15">
-        <f>(B22/(MIN(B14:B23)))*20</f>
-        <v>20.169743263314238</v>
+        <f>(B22/(MIN(B14:B23)))*18</f>
+        <v>20.870200287706098</v>
       </c>
     </row>
     <row r="23" spans="1:5">
       <c r="A23" s="14" t="s">
-        <v>50</v>
+        <v>40</v>
       </c>
       <c r="B23" s="15">
-        <v>4713</v>
+        <v>9037</v>
       </c>
       <c r="C23" s="15">
-        <f t="shared" si="1"/>
+        <f>(C22+3)</f>
         <v>30</v>
       </c>
-      <c r="D23" s="15"/>
+      <c r="D23" s="16"/>
       <c r="E23" s="15">
-        <f>(B23/(MIN(B14:B23)))*20</f>
-        <v>20</v>
+        <f>(B23/(MIN(B14:B23)))*18</f>
+        <v>18</v>
       </c>
     </row>
     <row r="25" spans="1:5">
       <c r="A25" s="17" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B25" s="17" t="s">
         <v>11</v>
@@ -2780,26 +2739,26 @@
     </row>
     <row r="26" spans="1:5">
       <c r="A26" s="14" t="s">
-        <v>73</v>
+        <v>41</v>
       </c>
       <c r="B26" s="15">
-        <v>18434</v>
+        <v>8886</v>
       </c>
       <c r="C26" s="15">
         <v>3</v>
       </c>
       <c r="D26" s="15"/>
       <c r="E26" s="15">
-        <f>(B26/(MIN(B26:B34)))*15</f>
-        <v>104.61975028376844</v>
+        <f>(B26/(MIN(B26:B35)))*20</f>
+        <v>37.708465945257799</v>
       </c>
     </row>
     <row r="27" spans="1:5">
       <c r="A27" s="14" t="s">
-        <v>71</v>
+        <v>48</v>
       </c>
       <c r="B27" s="15">
-        <v>4303</v>
+        <v>6520</v>
       </c>
       <c r="C27" s="15">
         <f>(C26+3)</f>
@@ -2807,136 +2766,138 @@
       </c>
       <c r="D27" s="15"/>
       <c r="E27" s="15">
-        <f>(B27/(MIN(B26:B34)))*20</f>
-        <v>32.561483163072268</v>
+        <f>(B27/(MIN(B26:B35)))*20</f>
+        <v>27.668151920220666</v>
       </c>
     </row>
     <row r="28" spans="1:5">
       <c r="A28" s="14" t="s">
-        <v>72</v>
+        <v>42</v>
       </c>
       <c r="B28" s="15">
-        <v>4259</v>
+        <v>5821</v>
       </c>
       <c r="C28" s="15">
-        <f t="shared" ref="C28:C33" si="2">(C27+3)</f>
+        <f t="shared" ref="C28:C34" si="1">(C27+3)</f>
         <v>9</v>
       </c>
       <c r="D28" s="15"/>
       <c r="E28" s="15">
-        <f>(B28/(MIN(B26:B34)))*20</f>
-        <v>32.228528187665532</v>
+        <f>(B28/(MIN(B26:B35)))*20</f>
+        <v>24.701888393804371</v>
       </c>
     </row>
     <row r="29" spans="1:5">
       <c r="A29" s="14" t="s">
-        <v>64</v>
+        <v>43</v>
       </c>
       <c r="B29" s="15">
-        <v>4152</v>
+        <v>5694</v>
       </c>
       <c r="C29" s="15">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>12</v>
       </c>
       <c r="D29" s="15"/>
       <c r="E29" s="15">
-        <f>(B29/(MIN(B26:B34)))*20</f>
-        <v>31.418842224744608</v>
+        <f>(B29/(MIN(B26:B35)))*20</f>
+        <v>24.162953532781664</v>
       </c>
     </row>
     <row r="30" spans="1:5">
       <c r="A30" s="14" t="s">
-        <v>65</v>
+        <v>44</v>
       </c>
       <c r="B30" s="15">
-        <v>3639</v>
+        <v>5456</v>
       </c>
       <c r="C30" s="15">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>15</v>
       </c>
       <c r="D30" s="15"/>
       <c r="E30" s="15">
-        <f>(B30/(MIN(B26:B34)))*20</f>
-        <v>27.536889897843363</v>
+        <f>(B30/(MIN(B26:B35)))*20</f>
+        <v>23.152981116061959</v>
       </c>
     </row>
     <row r="31" spans="1:5">
       <c r="A31" s="14" t="s">
-        <v>66</v>
+        <v>45</v>
       </c>
       <c r="B31" s="15">
-        <v>2801</v>
+        <v>5290</v>
       </c>
       <c r="C31" s="15">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>18</v>
       </c>
       <c r="D31" s="15"/>
       <c r="E31" s="15">
-        <f>(B31/(MIN(B26:B34)))*20</f>
-        <v>21.195611048051454</v>
+        <f>(B31/(MIN(B26:B35)))*20</f>
+        <v>22.448546573307873</v>
       </c>
     </row>
     <row r="32" spans="1:5">
       <c r="A32" s="14" t="s">
-        <v>67</v>
+        <v>46</v>
       </c>
       <c r="B32" s="15">
-        <v>2766</v>
+        <v>5110</v>
       </c>
       <c r="C32" s="15">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>21</v>
       </c>
       <c r="D32" s="15"/>
       <c r="E32" s="15">
-        <f>(B32/(MIN(B26:B34)))*20</f>
-        <v>20.930760499432463</v>
+        <f>(B32/(MIN(B26:B35)))*20</f>
+        <v>21.684701888393803</v>
       </c>
     </row>
     <row r="33" spans="1:5">
       <c r="A33" s="14" t="s">
-        <v>68</v>
+        <v>47</v>
       </c>
       <c r="B33" s="15">
-        <v>2730</v>
+        <v>4822</v>
       </c>
       <c r="C33" s="15">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>24</v>
       </c>
       <c r="D33" s="15"/>
       <c r="E33" s="15">
-        <f>(B33/(MIN(B26:B34)))*20</f>
-        <v>20.658342792281495</v>
+        <f>(B33/(MIN(B26:B35)))*20</f>
+        <v>20.462550392531295</v>
       </c>
     </row>
     <row r="34" spans="1:5">
       <c r="A34" s="14" t="s">
-        <v>70</v>
+        <v>49</v>
       </c>
       <c r="B34" s="15">
-        <v>2643</v>
+        <v>4753</v>
       </c>
       <c r="C34" s="15">
+        <f t="shared" si="1"/>
         <v>27</v>
       </c>
       <c r="D34" s="15"/>
       <c r="E34" s="15">
         <f>(B34/(MIN(B26:B35)))*20</f>
-        <v>21.797938144329898</v>
+        <v>20.169743263314238</v>
       </c>
     </row>
     <row r="35" spans="1:5">
       <c r="A35" s="14" t="s">
-        <v>110</v>
+        <v>50</v>
       </c>
       <c r="B35" s="15">
-        <v>2425</v>
+        <v>4713</v>
       </c>
       <c r="C35" s="15">
+        <f>(C34+3)</f>
         <v>30</v>
       </c>
       <c r="D35" s="15"/>
@@ -2946,132 +2907,246 @@
       </c>
     </row>
     <row r="37" spans="1:5">
-      <c r="B37" s="18"/>
+      <c r="A37" s="17" t="s">
+        <v>15</v>
+      </c>
+      <c r="B37" s="17" t="s">
+        <v>11</v>
+      </c>
+      <c r="C37" s="17" t="s">
+        <v>62</v>
+      </c>
+      <c r="D37" s="17" t="s">
+        <v>60</v>
+      </c>
+      <c r="E37" s="17"/>
     </row>
     <row r="38" spans="1:5">
-      <c r="B38" s="18"/>
+      <c r="A38" s="14" t="s">
+        <v>73</v>
+      </c>
+      <c r="B38" s="15">
+        <v>18434</v>
+      </c>
+      <c r="C38" s="15">
+        <v>3</v>
+      </c>
+      <c r="D38" s="15"/>
+      <c r="E38" s="15">
+        <f>(B38/(MIN(B38:B47)))*15</f>
+        <v>114.02474226804124</v>
+      </c>
     </row>
     <row r="39" spans="1:5">
-      <c r="B39" s="18"/>
+      <c r="A39" s="14" t="s">
+        <v>71</v>
+      </c>
+      <c r="B39" s="15">
+        <v>4303</v>
+      </c>
+      <c r="C39" s="15">
+        <f>(C38+3)</f>
+        <v>6</v>
+      </c>
+      <c r="D39" s="15"/>
+      <c r="E39" s="15">
+        <f>(B39/(MIN(B38:B47)))*20</f>
+        <v>35.488659793814435</v>
+      </c>
     </row>
     <row r="40" spans="1:5">
-      <c r="B40" s="18"/>
+      <c r="A40" s="14" t="s">
+        <v>72</v>
+      </c>
+      <c r="B40" s="15">
+        <v>4259</v>
+      </c>
+      <c r="C40" s="15">
+        <f t="shared" ref="C40:C45" si="2">(C39+3)</f>
+        <v>9</v>
+      </c>
+      <c r="D40" s="15"/>
+      <c r="E40" s="15">
+        <f>(B40/(MIN(B38:B47)))*20</f>
+        <v>35.125773195876292</v>
+      </c>
     </row>
     <row r="41" spans="1:5">
-      <c r="A41" t="s">
-        <v>111</v>
-      </c>
-      <c r="B41" s="18"/>
+      <c r="A41" s="14" t="s">
+        <v>64</v>
+      </c>
+      <c r="B41" s="15">
+        <v>4152</v>
+      </c>
+      <c r="C41" s="15">
+        <f t="shared" si="2"/>
+        <v>12</v>
+      </c>
+      <c r="D41" s="15"/>
+      <c r="E41" s="15">
+        <f>(B41/(MIN(B38:B47)))*20</f>
+        <v>34.243298969072164</v>
+      </c>
     </row>
     <row r="42" spans="1:5">
-      <c r="A42" t="s">
-        <v>112</v>
-      </c>
-      <c r="B42" s="18"/>
+      <c r="A42" s="14" t="s">
+        <v>65</v>
+      </c>
+      <c r="B42" s="15">
+        <v>3639</v>
+      </c>
+      <c r="C42" s="15">
+        <f t="shared" si="2"/>
+        <v>15</v>
+      </c>
+      <c r="D42" s="15"/>
+      <c r="E42" s="15">
+        <f>(B42/(MIN(B38:B47)))*20</f>
+        <v>30.012371134020619</v>
+      </c>
     </row>
     <row r="43" spans="1:5">
-      <c r="A43" t="s">
-        <v>113</v>
-      </c>
-      <c r="B43" s="18"/>
+      <c r="A43" s="14" t="s">
+        <v>66</v>
+      </c>
+      <c r="B43" s="15">
+        <v>2801</v>
+      </c>
+      <c r="C43" s="15">
+        <f t="shared" si="2"/>
+        <v>18</v>
+      </c>
+      <c r="D43" s="15"/>
+      <c r="E43" s="15">
+        <f>(B43/(MIN(B38:B47)))*20</f>
+        <v>23.101030927835051</v>
+      </c>
     </row>
     <row r="44" spans="1:5">
-      <c r="A44" t="s">
-        <v>114</v>
-      </c>
-      <c r="B44" s="18"/>
+      <c r="A44" s="14" t="s">
+        <v>67</v>
+      </c>
+      <c r="B44" s="15">
+        <v>2766</v>
+      </c>
+      <c r="C44" s="15">
+        <f t="shared" si="2"/>
+        <v>21</v>
+      </c>
+      <c r="D44" s="15"/>
+      <c r="E44" s="15">
+        <f>(B44/(MIN(B38:B47)))*20</f>
+        <v>22.812371134020619</v>
+      </c>
     </row>
     <row r="45" spans="1:5">
-      <c r="A45" t="s">
-        <v>115</v>
-      </c>
-      <c r="B45" s="18"/>
+      <c r="A45" s="14" t="s">
+        <v>68</v>
+      </c>
+      <c r="B45" s="15">
+        <v>2730</v>
+      </c>
+      <c r="C45" s="15">
+        <f t="shared" si="2"/>
+        <v>24</v>
+      </c>
+      <c r="D45" s="15"/>
+      <c r="E45" s="15">
+        <f>(B45/(MIN(B38:B47)))*20</f>
+        <v>22.515463917525771</v>
+      </c>
     </row>
     <row r="46" spans="1:5">
-      <c r="A46" t="s">
-        <v>116</v>
-      </c>
-      <c r="B46" s="18"/>
+      <c r="A46" s="14" t="s">
+        <v>70</v>
+      </c>
+      <c r="B46" s="15">
+        <v>2643</v>
+      </c>
+      <c r="C46" s="15">
+        <v>27</v>
+      </c>
+      <c r="D46" s="15"/>
+      <c r="E46" s="15">
+        <f>(B46/(MIN(B38:B47)))*20</f>
+        <v>21.797938144329898</v>
+      </c>
     </row>
     <row r="47" spans="1:5">
-      <c r="A47" t="s">
-        <v>117</v>
-      </c>
-      <c r="B47" s="18"/>
-    </row>
-    <row r="48" spans="1:5">
-      <c r="A48" t="s">
-        <v>118</v>
-      </c>
-      <c r="B48" s="18"/>
-    </row>
-    <row r="49" spans="1:2">
-      <c r="A49" t="s">
-        <v>119</v>
-      </c>
+      <c r="A47" s="14" t="s">
+        <v>110</v>
+      </c>
+      <c r="B47" s="15">
+        <v>2425</v>
+      </c>
+      <c r="C47" s="15">
+        <v>30</v>
+      </c>
+      <c r="D47" s="15"/>
+      <c r="E47" s="15">
+        <f>(B47/(MIN(B38:B47)))*20</f>
+        <v>20</v>
+      </c>
+    </row>
+    <row r="49" spans="2:2">
       <c r="B49" s="18"/>
     </row>
-    <row r="50" spans="1:2">
-      <c r="A50" t="s">
-        <v>120</v>
-      </c>
+    <row r="50" spans="2:2">
       <c r="B50" s="18"/>
     </row>
-    <row r="51" spans="1:2">
-      <c r="A51" t="s">
-        <v>121</v>
-      </c>
+    <row r="51" spans="2:2">
       <c r="B51" s="18"/>
     </row>
-    <row r="52" spans="1:2">
-      <c r="A52" t="s">
-        <v>122</v>
-      </c>
+    <row r="52" spans="2:2">
       <c r="B52" s="18"/>
     </row>
-    <row r="53" spans="1:2">
-      <c r="A53" t="s">
-        <v>123</v>
-      </c>
+    <row r="53" spans="2:2">
       <c r="B53" s="18"/>
     </row>
-    <row r="54" spans="1:2">
-      <c r="A54" t="s">
-        <v>124</v>
-      </c>
+    <row r="54" spans="2:2">
       <c r="B54" s="18"/>
     </row>
-    <row r="55" spans="1:2">
-      <c r="A55" t="s">
-        <v>125</v>
-      </c>
+    <row r="55" spans="2:2">
       <c r="B55" s="18"/>
     </row>
-    <row r="56" spans="1:2">
-      <c r="A56" t="s">
-        <v>126</v>
-      </c>
+    <row r="56" spans="2:2">
       <c r="B56" s="18"/>
     </row>
-    <row r="57" spans="1:2">
-      <c r="A57" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="58" spans="1:2">
-      <c r="A58" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="59" spans="1:2">
-      <c r="A59" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="60" spans="1:2">
-      <c r="A60" t="s">
-        <v>130</v>
-      </c>
+    <row r="57" spans="2:2">
+      <c r="B57" s="18"/>
+    </row>
+    <row r="58" spans="2:2">
+      <c r="B58" s="18"/>
+    </row>
+    <row r="59" spans="2:2">
+      <c r="B59" s="18"/>
+    </row>
+    <row r="60" spans="2:2">
+      <c r="B60" s="18"/>
+    </row>
+    <row r="61" spans="2:2">
+      <c r="B61" s="18"/>
+    </row>
+    <row r="62" spans="2:2">
+      <c r="B62" s="18"/>
+    </row>
+    <row r="63" spans="2:2">
+      <c r="B63" s="18"/>
+    </row>
+    <row r="64" spans="2:2">
+      <c r="B64" s="18"/>
+    </row>
+    <row r="65" spans="2:2">
+      <c r="B65" s="18"/>
+    </row>
+    <row r="66" spans="2:2">
+      <c r="B66" s="18"/>
+    </row>
+    <row r="67" spans="2:2">
+      <c r="B67" s="18"/>
+    </row>
+    <row r="68" spans="2:2">
+      <c r="B68" s="18"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>